<commit_message>
Actualización de automatizaciones UI (búsqueda visual y lógica de pegado RTF) y script de detección de patologías IA
</commit_message>
<xml_diff>
--- a/reporte_patologias.xlsx
+++ b/reporte_patologias.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,13 +487,6 @@
           <t>patologia_detectada</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>22</v>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -533,7 +526,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -553,7 +546,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -564,7 +557,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0%</t>
         </is>
       </c>
     </row>
@@ -576,7 +569,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2026-01-18 21:14:58</t>
+          <t>2026-02-06 05:27:12</t>
         </is>
       </c>
     </row>

</xml_diff>